<commit_message>
a couple of accounts got added
</commit_message>
<xml_diff>
--- a/white_internet.xlsx
+++ b/white_internet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="740">
   <si>
     <t xml:space="preserve">@aliasghar_1999</t>
   </si>
@@ -2904,6 +2904,18 @@
   </si>
   <si>
     <t xml:space="preserve">mostafa.pournasiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Masoumeh_Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@fereshte_aminy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تمنای وصال</t>
   </si>
 </sst>
 </file>
@@ -2997,7 +3009,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3028,6 +3040,14 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3161,10 +3181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F290"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C290" activeCellId="0" sqref="C290"/>
+      <selection pane="topLeft" activeCell="C289" activeCellId="0" sqref="C289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8644,7 +8664,7 @@
       <c r="E288" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F288" s="0" t="n">
+      <c r="F288" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8664,7 +8684,7 @@
       <c r="E289" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="F289" s="0" t="n">
+      <c r="F289" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8684,7 +8704,47 @@
       <c r="E290" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F290" s="0" t="n">
+      <c r="F290" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A291" s="10" t="s">
+        <v>736</v>
+      </c>
+      <c r="B291" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="C291" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D291" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E291" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F291" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B292" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="C292" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D292" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E292" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F292" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a self reported account got added
</commit_message>
<xml_diff>
--- a/white_internet.xlsx
+++ b/white_internet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="1046">
   <si>
     <t xml:space="preserve">@aliasghar_1999</t>
   </si>
@@ -3805,6 +3805,18 @@
   </si>
   <si>
     <t xml:space="preserve">نَفَس دُخت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@asemanihonar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">راحیل‏ 𓂆‌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@n_nikjoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIMA NIKJOO</t>
   </si>
 </sst>
 </file>
@@ -4070,10 +4082,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F439"/>
+  <dimension ref="A1:F441"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A419" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F439" activeCellId="0" sqref="F439"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A411" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F429" activeCellId="0" sqref="F429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12503,6 +12515,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A440" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B440" s="10" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C440" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="D440" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E440" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F440" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A441" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B441" s="10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C441" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D441" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="E441" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F441" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
a couple dozen of accounts got added
</commit_message>
<xml_diff>
--- a/white_internet.xlsx
+++ b/white_internet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="1137">
   <si>
     <t xml:space="preserve">@aliasghar_1999</t>
   </si>
@@ -3817,6 +3817,279 @@
   </si>
   <si>
     <t xml:space="preserve">NIMA NIKJOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@amirebtehaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amir Ebtehaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@irancell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTN Irancell-ایرانسل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@explorerr2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@saryeh_komala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozhda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Russell_Adlere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shah®ukh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@a_1874ba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">امیر ب ۷۴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@navidaaaaaaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navid mohammadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@yazecoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yazeco.ir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@amir_karimzad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amir Karimzad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@yasi_r_313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">یاسی رزاقیان اکانت قبلی ساسپندشد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@b_abbasiarand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bijan Abbasi Arand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@zarghami_ez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سید عزت الله ضرغامی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@dotone_channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DotOne دات‌وان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mmhhssnn7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کوروتوپول بهداشتی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@msteerpo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ghadirinetwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">احمد قدیری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@soheil_asaad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سهیل اسعد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@alirahimi1400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali Rahimi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@shaqayeqhastamm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شَ قایق</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ilam_98_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| دختر آلامتو |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@zeynabbahmani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زینب بهمنی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@amin2709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">امین</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Totya54442074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توتیا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@neda_andi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ندای اندیمشک</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@f_gholami1359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فاطمه غلامی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@farhad_nazarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فرهاد نظریان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@atefeh1127713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atefeh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@xuser44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@MmJmMmAmZV110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دیوُ دِلبَر(قلب مقاومتغَزِّة)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Doovare_Loor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دُووَرِ لُر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@faezem13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">𝒇𝒂𝒆𝒛𝒆 𝒎𝒂𝒅𝒂𝒅𝒊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@goldasteh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گلدسته</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@B_larde5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|•بـــاݩۅۍلـَردِه•|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@rana_1267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رعنـــآ:)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@hassan045081070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hassan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@zttabrizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zahra tabrizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Kh_amini13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">خانم امینی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ilqar1607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehdi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mehrdwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehrdad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@v_digar_hich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سوز سرما</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@moalem70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">معلم دهه هفتادی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@sarafakourii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سارا فکوری</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mamad__p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ممد پی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@gizBaBa4145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قیز بابا :) </t>
   </si>
 </sst>
 </file>
@@ -3910,7 +4183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3957,6 +4230,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4082,15 +4359,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F441"/>
+  <dimension ref="A1:F485"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A411" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F429" activeCellId="0" sqref="F429"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="G1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.69"/>
@@ -9636,16 +9913,16 @@
       <c r="A292" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="B292" s="10" t="s">
+      <c r="B292" s="8" t="s">
         <v>739</v>
       </c>
       <c r="C292" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E292" s="11" t="s">
+      <c r="E292" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F292" s="0" t="n">
+      <c r="F292" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9653,19 +9930,19 @@
       <c r="A293" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="B293" s="10" t="s">
+      <c r="B293" s="8" t="s">
         <v>741</v>
       </c>
       <c r="C293" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D293" s="11" t="s">
+      <c r="D293" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="E293" s="11" t="s">
+      <c r="E293" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F293" s="0" t="n">
+      <c r="F293" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9673,33 +9950,33 @@
       <c r="A294" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="B294" s="10" t="s">
+      <c r="B294" s="8" t="s">
         <v>743</v>
       </c>
       <c r="C294" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E294" s="11" t="s">
+      <c r="E294" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="F294" s="0" t="n">
+      <c r="F294" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A295" s="10" t="s">
+      <c r="A295" s="8" t="s">
         <v>744</v>
       </c>
-      <c r="B295" s="10" t="s">
+      <c r="B295" s="8" t="s">
         <v>745</v>
       </c>
       <c r="C295" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E295" s="11" t="s">
+      <c r="E295" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F295" s="0" t="n">
+      <c r="F295" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9707,19 +9984,19 @@
       <c r="A296" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B296" s="10" t="s">
+      <c r="B296" s="8" t="s">
         <v>747</v>
       </c>
       <c r="C296" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D296" s="11" t="s">
+      <c r="D296" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="E296" s="11" t="s">
+      <c r="E296" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="F296" s="0" t="n">
+      <c r="F296" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9727,19 +10004,19 @@
       <c r="A297" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B297" s="10" t="s">
+      <c r="B297" s="8" t="s">
         <v>749</v>
       </c>
       <c r="C297" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D297" s="11" t="s">
+      <c r="D297" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E297" s="11" t="s">
+      <c r="E297" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F297" s="0" t="n">
+      <c r="F297" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9747,19 +10024,19 @@
       <c r="A298" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="B298" s="10" t="s">
+      <c r="B298" s="8" t="s">
         <v>751</v>
       </c>
       <c r="C298" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D298" s="11" t="s">
+      <c r="D298" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E298" s="11" t="s">
+      <c r="E298" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F298" s="0" t="n">
+      <c r="F298" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9767,19 +10044,19 @@
       <c r="A299" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="B299" s="10" t="s">
+      <c r="B299" s="8" t="s">
         <v>753</v>
       </c>
       <c r="C299" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D299" s="11" t="s">
+      <c r="D299" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E299" s="11" t="s">
+      <c r="E299" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F299" s="0" t="n">
+      <c r="F299" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9787,19 +10064,19 @@
       <c r="A300" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="B300" s="10" t="s">
+      <c r="B300" s="8" t="s">
         <v>755</v>
       </c>
       <c r="C300" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D300" s="11" t="s">
+      <c r="D300" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="E300" s="11" t="s">
+      <c r="E300" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F300" s="0" t="n">
+      <c r="F300" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9807,19 +10084,19 @@
       <c r="A301" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="B301" s="10" t="s">
+      <c r="B301" s="8" t="s">
         <v>757</v>
       </c>
       <c r="C301" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D301" s="11" t="s">
+      <c r="D301" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E301" s="11" t="s">
+      <c r="E301" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F301" s="0" t="n">
+      <c r="F301" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9827,19 +10104,19 @@
       <c r="A302" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="B302" s="10" t="s">
+      <c r="B302" s="8" t="s">
         <v>759</v>
       </c>
       <c r="C302" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D302" s="11" t="s">
+      <c r="D302" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E302" s="11" t="s">
+      <c r="E302" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="F302" s="0" t="n">
+      <c r="F302" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9847,19 +10124,19 @@
       <c r="A303" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="B303" s="10" t="s">
+      <c r="B303" s="8" t="s">
         <v>761</v>
       </c>
       <c r="C303" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D303" s="11" t="s">
+      <c r="D303" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="E303" s="11" t="s">
+      <c r="E303" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="F303" s="0" t="n">
+      <c r="F303" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9867,17 +10144,17 @@
       <c r="A304" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="B304" s="10" t="s">
+      <c r="B304" s="8" t="s">
         <v>763</v>
       </c>
       <c r="C304" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D304" s="11"/>
-      <c r="E304" s="11" t="s">
+      <c r="D304" s="9"/>
+      <c r="E304" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F304" s="0" t="n">
+      <c r="F304" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9885,19 +10162,19 @@
       <c r="A305" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="B305" s="10" t="s">
+      <c r="B305" s="8" t="s">
         <v>765</v>
       </c>
       <c r="C305" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D305" s="11" t="s">
+      <c r="D305" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="E305" s="11" t="s">
+      <c r="E305" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="F305" s="0" t="n">
+      <c r="F305" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9905,19 +10182,19 @@
       <c r="A306" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="B306" s="10" t="s">
+      <c r="B306" s="8" t="s">
         <v>767</v>
       </c>
       <c r="C306" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D306" s="11" t="s">
+      <c r="D306" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E306" s="11" t="s">
+      <c r="E306" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="F306" s="0" t="n">
+      <c r="F306" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9925,19 +10202,19 @@
       <c r="A307" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="B307" s="10" t="s">
+      <c r="B307" s="8" t="s">
         <v>769</v>
       </c>
       <c r="C307" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D307" s="11" t="s">
+      <c r="D307" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E307" s="11" t="s">
+      <c r="E307" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F307" s="0" t="n">
+      <c r="F307" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9945,19 +10222,19 @@
       <c r="A308" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="B308" s="10" t="s">
+      <c r="B308" s="8" t="s">
         <v>771</v>
       </c>
       <c r="C308" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D308" s="11" t="s">
+      <c r="D308" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E308" s="11" t="s">
+      <c r="E308" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F308" s="0" t="n">
+      <c r="F308" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9965,39 +10242,39 @@
       <c r="A309" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="B309" s="10" t="s">
+      <c r="B309" s="8" t="s">
         <v>773</v>
       </c>
       <c r="C309" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D309" s="11" t="s">
+      <c r="D309" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E309" s="11" t="s">
+      <c r="E309" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F309" s="0" t="n">
+      <c r="F309" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A310" s="10" t="s">
+      <c r="A310" s="8" t="s">
         <v>774</v>
       </c>
-      <c r="B310" s="10" t="s">
+      <c r="B310" s="8" t="s">
         <v>775</v>
       </c>
       <c r="C310" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D310" s="11" t="s">
+      <c r="D310" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E310" s="11" t="s">
+      <c r="E310" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="F310" s="0" t="n">
+      <c r="F310" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10005,16 +10282,16 @@
       <c r="A311" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="B311" s="10" t="s">
+      <c r="B311" s="8" t="s">
         <v>777</v>
       </c>
       <c r="C311" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E311" s="11" t="s">
+      <c r="E311" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F311" s="0" t="n">
+      <c r="F311" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10022,19 +10299,19 @@
       <c r="A312" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="B312" s="10" t="s">
+      <c r="B312" s="8" t="s">
         <v>779</v>
       </c>
       <c r="C312" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D312" s="11" t="s">
+      <c r="D312" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="E312" s="11" t="s">
+      <c r="E312" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="F312" s="0" t="n">
+      <c r="F312" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10042,19 +10319,19 @@
       <c r="A313" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="B313" s="10" t="s">
+      <c r="B313" s="8" t="s">
         <v>781</v>
       </c>
       <c r="C313" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D313" s="11" t="s">
+      <c r="D313" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="E313" s="11" t="s">
+      <c r="E313" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="F313" s="0" t="n">
+      <c r="F313" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10062,19 +10339,19 @@
       <c r="A314" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="B314" s="10" t="s">
+      <c r="B314" s="8" t="s">
         <v>783</v>
       </c>
       <c r="C314" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D314" s="11" t="s">
+      <c r="D314" s="9" t="s">
         <v>784</v>
       </c>
-      <c r="E314" s="11" t="s">
+      <c r="E314" s="9" t="s">
         <v>784</v>
       </c>
-      <c r="F314" s="0" t="n">
+      <c r="F314" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10082,16 +10359,16 @@
       <c r="A315" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="B315" s="10" t="s">
+      <c r="B315" s="8" t="s">
         <v>786</v>
       </c>
       <c r="C315" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E315" s="11" t="s">
+      <c r="E315" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="F315" s="0" t="n">
+      <c r="F315" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10099,16 +10376,16 @@
       <c r="A316" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="B316" s="10" t="s">
+      <c r="B316" s="8" t="s">
         <v>788</v>
       </c>
       <c r="C316" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E316" s="11" t="s">
+      <c r="E316" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F316" s="0" t="n">
+      <c r="F316" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10116,39 +10393,39 @@
       <c r="A317" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="B317" s="10" t="s">
+      <c r="B317" s="8" t="s">
         <v>790</v>
       </c>
       <c r="C317" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D317" s="11" t="s">
+      <c r="D317" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E317" s="11" t="s">
+      <c r="E317" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F317" s="0" t="n">
+      <c r="F317" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A318" s="10" t="s">
+      <c r="A318" s="8" t="s">
         <v>791</v>
       </c>
-      <c r="B318" s="10" t="s">
+      <c r="B318" s="8" t="s">
         <v>792</v>
       </c>
       <c r="C318" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D318" s="11" t="s">
+      <c r="D318" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E318" s="11" t="s">
+      <c r="E318" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="F318" s="0" t="n">
+      <c r="F318" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10156,19 +10433,19 @@
       <c r="A319" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="B319" s="10" t="s">
+      <c r="B319" s="8" t="s">
         <v>794</v>
       </c>
       <c r="C319" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D319" s="11" t="s">
+      <c r="D319" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="E319" s="11" t="s">
+      <c r="E319" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F319" s="0" t="n">
+      <c r="F319" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10176,19 +10453,19 @@
       <c r="A320" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="B320" s="10" t="s">
+      <c r="B320" s="8" t="s">
         <v>796</v>
       </c>
       <c r="C320" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D320" s="11" t="s">
+      <c r="D320" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E320" s="11" t="s">
+      <c r="E320" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="F320" s="0" t="n">
+      <c r="F320" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10196,19 +10473,19 @@
       <c r="A321" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="B321" s="10" t="s">
+      <c r="B321" s="8" t="s">
         <v>798</v>
       </c>
       <c r="C321" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D321" s="11" t="s">
+      <c r="D321" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="E321" s="11" t="s">
+      <c r="E321" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F321" s="0" t="n">
+      <c r="F321" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10216,19 +10493,19 @@
       <c r="A322" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="B322" s="10" t="s">
+      <c r="B322" s="8" t="s">
         <v>800</v>
       </c>
       <c r="C322" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D322" s="11" t="s">
+      <c r="D322" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E322" s="11" t="s">
+      <c r="E322" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F322" s="0" t="n">
+      <c r="F322" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10236,19 +10513,19 @@
       <c r="A323" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="B323" s="10" t="s">
+      <c r="B323" s="8" t="s">
         <v>802</v>
       </c>
       <c r="C323" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D323" s="11" t="s">
+      <c r="D323" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E323" s="11" t="s">
+      <c r="E323" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F323" s="0" t="n">
+      <c r="F323" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10256,19 +10533,19 @@
       <c r="A324" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="B324" s="10" t="s">
+      <c r="B324" s="8" t="s">
         <v>804</v>
       </c>
       <c r="C324" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D324" s="11" t="s">
+      <c r="D324" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E324" s="11" t="s">
+      <c r="E324" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F324" s="0" t="n">
+      <c r="F324" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10276,19 +10553,19 @@
       <c r="A325" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="B325" s="10" t="s">
+      <c r="B325" s="8" t="s">
         <v>806</v>
       </c>
       <c r="C325" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D325" s="11" t="s">
+      <c r="D325" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E325" s="11" t="s">
+      <c r="E325" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F325" s="0" t="n">
+      <c r="F325" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10296,16 +10573,16 @@
       <c r="A326" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="B326" s="10" t="s">
+      <c r="B326" s="8" t="s">
         <v>808</v>
       </c>
       <c r="C326" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E326" s="11" t="s">
+      <c r="E326" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F326" s="0" t="n">
+      <c r="F326" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10313,19 +10590,19 @@
       <c r="A327" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="B327" s="10" t="s">
+      <c r="B327" s="8" t="s">
         <v>810</v>
       </c>
       <c r="C327" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D327" s="11" t="s">
+      <c r="D327" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="E327" s="11" t="s">
+      <c r="E327" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F327" s="0" t="n">
+      <c r="F327" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10333,19 +10610,19 @@
       <c r="A328" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="B328" s="10" t="s">
+      <c r="B328" s="8" t="s">
         <v>812</v>
       </c>
       <c r="C328" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D328" s="11" t="s">
+      <c r="D328" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="E328" s="11" t="s">
+      <c r="E328" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F328" s="0" t="n">
+      <c r="F328" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10353,19 +10630,19 @@
       <c r="A329" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="B329" s="10" t="s">
+      <c r="B329" s="8" t="s">
         <v>814</v>
       </c>
       <c r="C329" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D329" s="11" t="s">
+      <c r="D329" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E329" s="11" t="s">
+      <c r="E329" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F329" s="0" t="n">
+      <c r="F329" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10373,19 +10650,19 @@
       <c r="A330" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="B330" s="10" t="s">
+      <c r="B330" s="8" t="s">
         <v>816</v>
       </c>
       <c r="C330" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D330" s="11" t="s">
+      <c r="D330" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="E330" s="11" t="s">
+      <c r="E330" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F330" s="0" t="n">
+      <c r="F330" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10393,19 +10670,19 @@
       <c r="A331" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="B331" s="10" t="s">
+      <c r="B331" s="8" t="s">
         <v>818</v>
       </c>
       <c r="C331" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D331" s="11" t="s">
+      <c r="D331" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="E331" s="11" t="s">
+      <c r="E331" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F331" s="0" t="n">
+      <c r="F331" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10413,19 +10690,19 @@
       <c r="A332" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="B332" s="10" t="s">
+      <c r="B332" s="8" t="s">
         <v>310</v>
       </c>
       <c r="C332" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D332" s="11" t="s">
+      <c r="D332" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="E332" s="11" t="s">
+      <c r="E332" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="F332" s="0" t="n">
+      <c r="F332" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10433,19 +10710,19 @@
       <c r="A333" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="B333" s="10" t="s">
+      <c r="B333" s="8" t="s">
         <v>821</v>
       </c>
       <c r="C333" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D333" s="11" t="s">
+      <c r="D333" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E333" s="11" t="s">
+      <c r="E333" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="F333" s="0" t="n">
+      <c r="F333" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10453,19 +10730,19 @@
       <c r="A334" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="B334" s="10" t="s">
+      <c r="B334" s="8" t="s">
         <v>823</v>
       </c>
       <c r="C334" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D334" s="11" t="s">
+      <c r="D334" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E334" s="11" t="s">
+      <c r="E334" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F334" s="0" t="n">
+      <c r="F334" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10473,19 +10750,19 @@
       <c r="A335" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="B335" s="10" t="s">
+      <c r="B335" s="8" t="s">
         <v>825</v>
       </c>
       <c r="C335" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D335" s="11" t="s">
+      <c r="D335" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E335" s="11" t="s">
+      <c r="E335" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F335" s="0" t="n">
+      <c r="F335" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10499,13 +10776,13 @@
       <c r="C336" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D336" s="11" t="s">
+      <c r="D336" s="9" t="s">
         <v>828</v>
       </c>
       <c r="E336" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F336" s="0" t="n">
+      <c r="F336" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10513,19 +10790,19 @@
       <c r="A337" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="B337" s="10" t="s">
+      <c r="B337" s="8" t="s">
         <v>830</v>
       </c>
       <c r="C337" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D337" s="11" t="s">
+      <c r="D337" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E337" s="11" t="s">
+      <c r="E337" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="F337" s="0" t="n">
+      <c r="F337" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10533,19 +10810,19 @@
       <c r="A338" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="B338" s="10" t="s">
+      <c r="B338" s="8" t="s">
         <v>832</v>
       </c>
       <c r="C338" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D338" s="11" t="s">
+      <c r="D338" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="E338" s="11" t="s">
+      <c r="E338" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="F338" s="0" t="n">
+      <c r="F338" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10553,19 +10830,19 @@
       <c r="A339" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="B339" s="10" t="s">
+      <c r="B339" s="8" t="s">
         <v>834</v>
       </c>
       <c r="C339" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D339" s="11" t="s">
+      <c r="D339" s="9" t="s">
         <v>784</v>
       </c>
-      <c r="E339" s="11" t="s">
+      <c r="E339" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="F339" s="0" t="n">
+      <c r="F339" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10573,19 +10850,19 @@
       <c r="A340" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="B340" s="10" t="s">
+      <c r="B340" s="8" t="s">
         <v>837</v>
       </c>
       <c r="C340" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D340" s="11" t="s">
+      <c r="D340" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E340" s="11" t="s">
+      <c r="E340" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F340" s="0" t="n">
+      <c r="F340" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10593,19 +10870,19 @@
       <c r="A341" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="B341" s="10" t="s">
+      <c r="B341" s="8" t="s">
         <v>839</v>
       </c>
       <c r="C341" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D341" s="11" t="s">
+      <c r="D341" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E341" s="11" t="s">
+      <c r="E341" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F341" s="0" t="n">
+      <c r="F341" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10613,19 +10890,19 @@
       <c r="A342" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="B342" s="10" t="s">
+      <c r="B342" s="8" t="s">
         <v>841</v>
       </c>
       <c r="C342" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D342" s="11" t="s">
+      <c r="D342" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E342" s="11" t="s">
+      <c r="E342" s="9" t="s">
         <v>842</v>
       </c>
-      <c r="F342" s="0" t="n">
+      <c r="F342" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10633,19 +10910,19 @@
       <c r="A343" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="B343" s="10" t="s">
+      <c r="B343" s="8" t="s">
         <v>844</v>
       </c>
       <c r="C343" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D343" s="11" t="s">
+      <c r="D343" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E343" s="11" t="s">
+      <c r="E343" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F343" s="0" t="n">
+      <c r="F343" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10659,13 +10936,13 @@
       <c r="C344" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D344" s="11" t="s">
+      <c r="D344" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="E344" s="11" t="s">
+      <c r="E344" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="F344" s="0" t="n">
+      <c r="F344" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10673,19 +10950,19 @@
       <c r="A345" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="B345" s="10" t="s">
+      <c r="B345" s="8" t="s">
         <v>849</v>
       </c>
       <c r="C345" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D345" s="11" t="s">
+      <c r="D345" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="E345" s="11" t="s">
+      <c r="E345" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="F345" s="0" t="n">
+      <c r="F345" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10693,16 +10970,16 @@
       <c r="A346" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="B346" s="10" t="s">
+      <c r="B346" s="8" t="s">
         <v>851</v>
       </c>
       <c r="C346" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E346" s="11" t="s">
+      <c r="E346" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F346" s="0" t="n">
+      <c r="F346" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10710,16 +10987,16 @@
       <c r="A347" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="B347" s="10" t="s">
+      <c r="B347" s="8" t="s">
         <v>853</v>
       </c>
       <c r="C347" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E347" s="11" t="s">
+      <c r="E347" s="9" t="s">
         <v>854</v>
       </c>
-      <c r="F347" s="0" t="n">
+      <c r="F347" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10727,19 +11004,19 @@
       <c r="A348" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="B348" s="10" t="s">
+      <c r="B348" s="8" t="s">
         <v>856</v>
       </c>
       <c r="C348" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D348" s="11" t="s">
+      <c r="D348" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E348" s="11" t="s">
+      <c r="E348" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F348" s="0" t="n">
+      <c r="F348" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10747,19 +11024,19 @@
       <c r="A349" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="B349" s="10" t="s">
+      <c r="B349" s="8" t="s">
         <v>858</v>
       </c>
       <c r="C349" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D349" s="11" t="s">
+      <c r="D349" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E349" s="11" t="s">
+      <c r="E349" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="F349" s="0" t="n">
+      <c r="F349" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10767,16 +11044,16 @@
       <c r="A350" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="B350" s="10" t="s">
+      <c r="B350" s="8" t="s">
         <v>860</v>
       </c>
       <c r="C350" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E350" s="11" t="s">
+      <c r="E350" s="9" t="s">
         <v>861</v>
       </c>
-      <c r="F350" s="0" t="n">
+      <c r="F350" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10784,39 +11061,39 @@
       <c r="A351" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="B351" s="10" t="s">
+      <c r="B351" s="8" t="s">
         <v>863</v>
       </c>
       <c r="C351" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D351" s="11" t="s">
+      <c r="D351" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E351" s="11" t="s">
+      <c r="E351" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="F351" s="0" t="n">
+      <c r="F351" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A352" s="10" t="s">
+      <c r="A352" s="8" t="s">
         <v>864</v>
       </c>
-      <c r="B352" s="10" t="s">
+      <c r="B352" s="8" t="s">
         <v>865</v>
       </c>
       <c r="C352" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D352" s="11" t="s">
+      <c r="D352" s="9" t="s">
         <v>866</v>
       </c>
-      <c r="E352" s="11" t="s">
+      <c r="E352" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F352" s="0" t="n">
+      <c r="F352" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10824,36 +11101,36 @@
       <c r="A353" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="B353" s="10" t="s">
+      <c r="B353" s="8" t="s">
         <v>868</v>
       </c>
       <c r="C353" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D353" s="11" t="s">
+      <c r="D353" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="E353" s="11" t="s">
+      <c r="E353" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="F353" s="0" t="n">
+      <c r="F353" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A354" s="10" t="s">
+      <c r="A354" s="8" t="s">
         <v>869</v>
       </c>
-      <c r="B354" s="10" t="s">
+      <c r="B354" s="8" t="s">
         <v>870</v>
       </c>
       <c r="C354" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E354" s="11" t="s">
+      <c r="E354" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F354" s="0" t="n">
+      <c r="F354" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10861,33 +11138,33 @@
       <c r="A355" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="B355" s="10" t="s">
+      <c r="B355" s="8" t="s">
         <v>872</v>
       </c>
       <c r="C355" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E355" s="11" t="s">
+      <c r="E355" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F355" s="0" t="n">
+      <c r="F355" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A356" s="10" t="s">
+      <c r="A356" s="8" t="s">
         <v>873</v>
       </c>
-      <c r="B356" s="10" t="s">
+      <c r="B356" s="8" t="s">
         <v>874</v>
       </c>
       <c r="C356" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E356" s="11" t="s">
+      <c r="E356" s="9" t="s">
         <v>875</v>
       </c>
-      <c r="F356" s="0" t="n">
+      <c r="F356" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10895,19 +11172,19 @@
       <c r="A357" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="B357" s="10" t="s">
+      <c r="B357" s="8" t="s">
         <v>877</v>
       </c>
       <c r="C357" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D357" s="11" t="s">
+      <c r="D357" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E357" s="11" t="s">
+      <c r="E357" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="F357" s="0" t="n">
+      <c r="F357" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10915,16 +11192,16 @@
       <c r="A358" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="B358" s="10" t="s">
+      <c r="B358" s="8" t="s">
         <v>879</v>
       </c>
       <c r="C358" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E358" s="11" t="s">
+      <c r="E358" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="F358" s="0" t="n">
+      <c r="F358" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10932,19 +11209,19 @@
       <c r="A359" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="B359" s="10" t="s">
+      <c r="B359" s="8" t="s">
         <v>881</v>
       </c>
-      <c r="C359" s="10" t="n">
+      <c r="C359" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D359" s="11" t="s">
+      <c r="D359" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E359" s="11" t="s">
+      <c r="E359" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F359" s="0" t="n">
+      <c r="F359" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10952,19 +11229,19 @@
       <c r="A360" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="B360" s="10" t="s">
+      <c r="B360" s="8" t="s">
         <v>883</v>
       </c>
       <c r="C360" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D360" s="11" t="s">
+      <c r="D360" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E360" s="11" t="s">
+      <c r="E360" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F360" s="0" t="n">
+      <c r="F360" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10972,19 +11249,19 @@
       <c r="A361" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="B361" s="10" t="s">
+      <c r="B361" s="8" t="s">
         <v>885</v>
       </c>
       <c r="C361" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D361" s="11" t="s">
+      <c r="D361" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E361" s="11" t="s">
+      <c r="E361" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="F361" s="0" t="n">
+      <c r="F361" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10992,19 +11269,19 @@
       <c r="A362" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="B362" s="10" t="s">
+      <c r="B362" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C362" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D362" s="11" t="s">
+      <c r="D362" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E362" s="11" t="s">
+      <c r="E362" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="F362" s="0" t="n">
+      <c r="F362" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11012,19 +11289,19 @@
       <c r="A363" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="B363" s="10" t="s">
+      <c r="B363" s="8" t="s">
         <v>888</v>
       </c>
       <c r="C363" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D363" s="11" t="s">
+      <c r="D363" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="E363" s="11" t="s">
+      <c r="E363" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="F363" s="0" t="n">
+      <c r="F363" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11032,19 +11309,19 @@
       <c r="A364" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="B364" s="10" t="s">
+      <c r="B364" s="8" t="s">
         <v>890</v>
       </c>
       <c r="C364" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D364" s="11" t="s">
+      <c r="D364" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E364" s="11" t="s">
+      <c r="E364" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F364" s="0" t="n">
+      <c r="F364" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11052,19 +11329,19 @@
       <c r="A365" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="B365" s="10" t="s">
+      <c r="B365" s="8" t="s">
         <v>892</v>
       </c>
       <c r="C365" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D365" s="11" t="s">
+      <c r="D365" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E365" s="11" t="s">
+      <c r="E365" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="F365" s="0" t="n">
+      <c r="F365" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11072,19 +11349,19 @@
       <c r="A366" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="B366" s="10" t="s">
+      <c r="B366" s="8" t="s">
         <v>894</v>
       </c>
       <c r="C366" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D366" s="11" t="s">
+      <c r="D366" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E366" s="11" t="s">
+      <c r="E366" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F366" s="0" t="n">
+      <c r="F366" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11092,19 +11369,19 @@
       <c r="A367" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="B367" s="10" t="s">
+      <c r="B367" s="8" t="s">
         <v>896</v>
       </c>
       <c r="C367" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D367" s="11" t="s">
+      <c r="D367" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="E367" s="11" t="s">
+      <c r="E367" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F367" s="0" t="n">
+      <c r="F367" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11112,19 +11389,19 @@
       <c r="A368" s="1" t="s">
         <v>897</v>
       </c>
-      <c r="B368" s="10" t="s">
+      <c r="B368" s="8" t="s">
         <v>898</v>
       </c>
       <c r="C368" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D368" s="11" t="s">
+      <c r="D368" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E368" s="11" t="s">
+      <c r="E368" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F368" s="0" t="n">
+      <c r="F368" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11132,19 +11409,19 @@
       <c r="A369" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="B369" s="10" t="s">
+      <c r="B369" s="8" t="s">
         <v>900</v>
       </c>
       <c r="C369" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D369" s="11" t="s">
+      <c r="D369" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="E369" s="11" t="s">
+      <c r="E369" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F369" s="0" t="n">
+      <c r="F369" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11152,19 +11429,19 @@
       <c r="A370" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="B370" s="10" t="s">
+      <c r="B370" s="8" t="s">
         <v>902</v>
       </c>
       <c r="C370" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D370" s="11" t="s">
+      <c r="D370" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E370" s="11" t="s">
+      <c r="E370" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F370" s="0" t="n">
+      <c r="F370" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11172,16 +11449,16 @@
       <c r="A371" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="B371" s="10" t="s">
+      <c r="B371" s="8" t="s">
         <v>904</v>
       </c>
       <c r="C371" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E371" s="11" t="s">
+      <c r="E371" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="F371" s="0" t="n">
+      <c r="F371" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11189,19 +11466,19 @@
       <c r="A372" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="B372" s="10" t="s">
+      <c r="B372" s="8" t="s">
         <v>906</v>
       </c>
       <c r="C372" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="D372" s="11" t="s">
+      <c r="D372" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E372" s="11" t="s">
+      <c r="E372" s="9" t="s">
         <v>866</v>
       </c>
-      <c r="F372" s="0" t="n">
+      <c r="F372" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11209,19 +11486,19 @@
       <c r="A373" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="B373" s="10" t="s">
+      <c r="B373" s="8" t="s">
         <v>908</v>
       </c>
       <c r="C373" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D373" s="11" t="s">
+      <c r="D373" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E373" s="11" t="s">
+      <c r="E373" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F373" s="0" t="n">
+      <c r="F373" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11229,19 +11506,19 @@
       <c r="A374" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="B374" s="10" t="s">
+      <c r="B374" s="8" t="s">
         <v>910</v>
       </c>
       <c r="C374" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D374" s="11" t="s">
+      <c r="D374" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E374" s="11" t="s">
+      <c r="E374" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F374" s="0" t="n">
+      <c r="F374" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11249,19 +11526,19 @@
       <c r="A375" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="B375" s="10" t="s">
+      <c r="B375" s="8" t="s">
         <v>912</v>
       </c>
       <c r="C375" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D375" s="11" t="s">
+      <c r="D375" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E375" s="11" t="s">
+      <c r="E375" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="F375" s="0" t="n">
+      <c r="F375" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11269,19 +11546,19 @@
       <c r="A376" s="1" t="s">
         <v>913</v>
       </c>
-      <c r="B376" s="10" t="s">
+      <c r="B376" s="8" t="s">
         <v>914</v>
       </c>
       <c r="C376" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D376" s="11" t="s">
+      <c r="D376" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="E376" s="11" t="s">
+      <c r="E376" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="F376" s="0" t="n">
+      <c r="F376" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11289,19 +11566,19 @@
       <c r="A377" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="B377" s="10" t="s">
+      <c r="B377" s="8" t="s">
         <v>916</v>
       </c>
       <c r="C377" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D377" s="11" t="s">
+      <c r="D377" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E377" s="11" t="s">
+      <c r="E377" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F377" s="0" t="n">
+      <c r="F377" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11309,16 +11586,16 @@
       <c r="A378" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="B378" s="10" t="s">
+      <c r="B378" s="8" t="s">
         <v>918</v>
       </c>
       <c r="C378" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E378" s="11" t="s">
+      <c r="E378" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F378" s="0" t="n">
+      <c r="F378" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11326,19 +11603,19 @@
       <c r="A379" s="1" t="s">
         <v>919</v>
       </c>
-      <c r="B379" s="10" t="s">
+      <c r="B379" s="8" t="s">
         <v>920</v>
       </c>
       <c r="C379" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D379" s="11" t="s">
+      <c r="D379" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E379" s="11" t="s">
+      <c r="E379" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F379" s="0" t="n">
+      <c r="F379" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11346,16 +11623,16 @@
       <c r="A380" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="B380" s="10" t="s">
+      <c r="B380" s="8" t="s">
         <v>922</v>
       </c>
       <c r="C380" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E380" s="11" t="s">
+      <c r="E380" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F380" s="0" t="n">
+      <c r="F380" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11363,19 +11640,19 @@
       <c r="A381" s="1" t="s">
         <v>923</v>
       </c>
-      <c r="B381" s="10" t="s">
+      <c r="B381" s="8" t="s">
         <v>924</v>
       </c>
       <c r="C381" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D381" s="11" t="s">
+      <c r="D381" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="E381" s="11" t="s">
+      <c r="E381" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="F381" s="0" t="n">
+      <c r="F381" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11383,19 +11660,19 @@
       <c r="A382" s="1" t="s">
         <v>925</v>
       </c>
-      <c r="B382" s="10" t="s">
+      <c r="B382" s="8" t="s">
         <v>926</v>
       </c>
       <c r="C382" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D382" s="11" t="s">
+      <c r="D382" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="E382" s="11" t="s">
+      <c r="E382" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="F382" s="0" t="n">
+      <c r="F382" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11403,19 +11680,19 @@
       <c r="A383" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="B383" s="10" t="s">
+      <c r="B383" s="8" t="s">
         <v>928</v>
       </c>
       <c r="C383" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D383" s="11" t="s">
+      <c r="D383" s="9" t="s">
         <v>676</v>
       </c>
-      <c r="E383" s="11" t="s">
+      <c r="E383" s="9" t="s">
         <v>676</v>
       </c>
-      <c r="F383" s="0" t="n">
+      <c r="F383" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11423,39 +11700,39 @@
       <c r="A384" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="B384" s="10" t="s">
+      <c r="B384" s="8" t="s">
         <v>930</v>
       </c>
       <c r="C384" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D384" s="11" t="s">
+      <c r="D384" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E384" s="11" t="s">
+      <c r="E384" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F384" s="0" t="n">
+      <c r="F384" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A385" s="10" t="s">
+      <c r="A385" s="8" t="s">
         <v>931</v>
       </c>
-      <c r="B385" s="10" t="s">
+      <c r="B385" s="8" t="s">
         <v>932</v>
       </c>
       <c r="C385" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D385" s="11" t="s">
+      <c r="D385" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="E385" s="11" t="s">
+      <c r="E385" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="F385" s="0" t="n">
+      <c r="F385" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11463,19 +11740,19 @@
       <c r="A386" s="1" t="s">
         <v>933</v>
       </c>
-      <c r="B386" s="10" t="s">
+      <c r="B386" s="8" t="s">
         <v>934</v>
       </c>
       <c r="C386" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D386" s="11" t="s">
+      <c r="D386" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="E386" s="11" t="s">
+      <c r="E386" s="9" t="s">
         <v>935</v>
       </c>
-      <c r="F386" s="0" t="n">
+      <c r="F386" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11483,19 +11760,19 @@
       <c r="A387" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="B387" s="10" t="s">
+      <c r="B387" s="8" t="s">
         <v>937</v>
       </c>
       <c r="C387" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D387" s="11" t="s">
+      <c r="D387" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="E387" s="11" t="s">
+      <c r="E387" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="F387" s="0" t="n">
+      <c r="F387" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11503,19 +11780,19 @@
       <c r="A388" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="B388" s="10" t="s">
+      <c r="B388" s="8" t="s">
         <v>939</v>
       </c>
       <c r="C388" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D388" s="11" t="s">
+      <c r="D388" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="E388" s="11" t="s">
+      <c r="E388" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="F388" s="0" t="n">
+      <c r="F388" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11523,16 +11800,16 @@
       <c r="A389" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="B389" s="10" t="s">
+      <c r="B389" s="8" t="s">
         <v>941</v>
       </c>
       <c r="C389" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E389" s="11" t="s">
+      <c r="E389" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="F389" s="0" t="n">
+      <c r="F389" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11540,19 +11817,19 @@
       <c r="A390" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="B390" s="10" t="s">
+      <c r="B390" s="8" t="s">
         <v>943</v>
       </c>
       <c r="C390" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D390" s="11" t="s">
+      <c r="D390" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E390" s="11" t="s">
+      <c r="E390" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="F390" s="0" t="n">
+      <c r="F390" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11560,16 +11837,16 @@
       <c r="A391" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="B391" s="10" t="s">
+      <c r="B391" s="8" t="s">
         <v>945</v>
       </c>
       <c r="C391" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E391" s="11" t="s">
+      <c r="E391" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="F391" s="0" t="n">
+      <c r="F391" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11577,19 +11854,19 @@
       <c r="A392" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="B392" s="10" t="s">
+      <c r="B392" s="8" t="s">
         <v>947</v>
       </c>
       <c r="C392" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D392" s="11" t="s">
+      <c r="D392" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E392" s="11" t="s">
+      <c r="E392" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F392" s="0" t="n">
+      <c r="F392" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11597,16 +11874,16 @@
       <c r="A393" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="B393" s="10" t="s">
+      <c r="B393" s="8" t="s">
         <v>949</v>
       </c>
       <c r="C393" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E393" s="11" t="s">
+      <c r="E393" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F393" s="0" t="n">
+      <c r="F393" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11614,19 +11891,19 @@
       <c r="A394" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="B394" s="10" t="s">
+      <c r="B394" s="8" t="s">
         <v>951</v>
       </c>
       <c r="C394" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D394" s="11" t="s">
+      <c r="D394" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="E394" s="11" t="s">
+      <c r="E394" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="F394" s="0" t="n">
+      <c r="F394" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11634,19 +11911,19 @@
       <c r="A395" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="B395" s="10" t="s">
+      <c r="B395" s="8" t="s">
         <v>953</v>
       </c>
       <c r="C395" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D395" s="11" t="s">
+      <c r="D395" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E395" s="11" t="s">
+      <c r="E395" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F395" s="0" t="n">
+      <c r="F395" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11654,19 +11931,19 @@
       <c r="A396" s="1" t="s">
         <v>954</v>
       </c>
-      <c r="B396" s="10" t="s">
+      <c r="B396" s="8" t="s">
         <v>955</v>
       </c>
       <c r="C396" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D396" s="11" t="s">
+      <c r="D396" s="9" t="s">
         <v>784</v>
       </c>
-      <c r="E396" s="11" t="s">
+      <c r="E396" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="F396" s="0" t="n">
+      <c r="F396" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11674,19 +11951,19 @@
       <c r="A397" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="B397" s="10" t="s">
+      <c r="B397" s="8" t="s">
         <v>957</v>
       </c>
       <c r="C397" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D397" s="11" t="s">
+      <c r="D397" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E397" s="11" t="s">
+      <c r="E397" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F397" s="0" t="n">
+      <c r="F397" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11694,19 +11971,19 @@
       <c r="A398" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="B398" s="10" t="s">
+      <c r="B398" s="8" t="s">
         <v>959</v>
       </c>
       <c r="C398" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D398" s="11" t="s">
+      <c r="D398" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E398" s="11" t="s">
+      <c r="E398" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F398" s="0" t="n">
+      <c r="F398" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11714,19 +11991,19 @@
       <c r="A399" s="1" t="s">
         <v>960</v>
       </c>
-      <c r="B399" s="10" t="s">
+      <c r="B399" s="8" t="s">
         <v>961</v>
       </c>
       <c r="C399" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D399" s="11" t="s">
+      <c r="D399" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E399" s="11" t="s">
+      <c r="E399" s="9" t="s">
         <v>724</v>
       </c>
-      <c r="F399" s="0" t="n">
+      <c r="F399" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11734,19 +12011,19 @@
       <c r="A400" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="B400" s="10" t="s">
+      <c r="B400" s="8" t="s">
         <v>963</v>
       </c>
       <c r="C400" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D400" s="11" t="s">
+      <c r="D400" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E400" s="11" t="s">
+      <c r="E400" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F400" s="0" t="n">
+      <c r="F400" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11754,16 +12031,16 @@
       <c r="A401" s="1" t="s">
         <v>964</v>
       </c>
-      <c r="B401" s="10" t="s">
+      <c r="B401" s="8" t="s">
         <v>965</v>
       </c>
       <c r="C401" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E401" s="11" t="s">
+      <c r="E401" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F401" s="0" t="n">
+      <c r="F401" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11771,19 +12048,19 @@
       <c r="A402" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="B402" s="10" t="s">
+      <c r="B402" s="8" t="s">
         <v>967</v>
       </c>
       <c r="C402" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D402" s="11" t="s">
+      <c r="D402" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E402" s="11" t="s">
+      <c r="E402" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="F402" s="0" t="n">
+      <c r="F402" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11791,19 +12068,19 @@
       <c r="A403" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="B403" s="10" t="s">
+      <c r="B403" s="8" t="s">
         <v>969</v>
       </c>
       <c r="C403" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D403" s="11" t="s">
+      <c r="D403" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E403" s="11" t="s">
+      <c r="E403" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F403" s="0" t="n">
+      <c r="F403" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11811,19 +12088,19 @@
       <c r="A404" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="B404" s="10" t="s">
+      <c r="B404" s="8" t="s">
         <v>971</v>
       </c>
       <c r="C404" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D404" s="11" t="s">
+      <c r="D404" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E404" s="11" t="s">
+      <c r="E404" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F404" s="0" t="n">
+      <c r="F404" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11831,19 +12108,19 @@
       <c r="A405" s="1" t="s">
         <v>972</v>
       </c>
-      <c r="B405" s="10" t="s">
+      <c r="B405" s="8" t="s">
         <v>973</v>
       </c>
       <c r="C405" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D405" s="11" t="s">
+      <c r="D405" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="E405" s="11" t="s">
+      <c r="E405" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="F405" s="0" t="n">
+      <c r="F405" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11851,19 +12128,19 @@
       <c r="A406" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="B406" s="10" t="s">
+      <c r="B406" s="8" t="s">
         <v>975</v>
       </c>
       <c r="C406" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D406" s="11" t="s">
+      <c r="D406" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="E406" s="11" t="s">
+      <c r="E406" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="F406" s="0" t="n">
+      <c r="F406" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11871,19 +12148,19 @@
       <c r="A407" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B407" s="10" t="s">
+      <c r="B407" s="8" t="s">
         <v>977</v>
       </c>
       <c r="C407" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D407" s="11" t="s">
+      <c r="D407" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E407" s="11" t="s">
+      <c r="E407" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F407" s="0" t="n">
+      <c r="F407" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11891,19 +12168,19 @@
       <c r="A408" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B408" s="10" t="s">
+      <c r="B408" s="8" t="s">
         <v>979</v>
       </c>
       <c r="C408" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D408" s="11" t="s">
+      <c r="D408" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E408" s="11" t="s">
+      <c r="E408" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F408" s="0" t="n">
+      <c r="F408" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11911,16 +12188,16 @@
       <c r="A409" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="B409" s="10" t="s">
+      <c r="B409" s="8" t="s">
         <v>981</v>
       </c>
       <c r="C409" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E409" s="11" t="s">
+      <c r="E409" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F409" s="0" t="n">
+      <c r="F409" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11928,19 +12205,19 @@
       <c r="A410" s="1" t="s">
         <v>982</v>
       </c>
-      <c r="B410" s="10" t="s">
+      <c r="B410" s="8" t="s">
         <v>983</v>
       </c>
       <c r="C410" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D410" s="11" t="s">
+      <c r="D410" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="E410" s="11" t="s">
+      <c r="E410" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="F410" s="0" t="n">
+      <c r="F410" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11948,19 +12225,19 @@
       <c r="A411" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="B411" s="10" t="s">
+      <c r="B411" s="8" t="s">
         <v>985</v>
       </c>
       <c r="C411" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D411" s="11" t="s">
+      <c r="D411" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E411" s="11" t="s">
+      <c r="E411" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F411" s="0" t="n">
+      <c r="F411" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11968,19 +12245,19 @@
       <c r="A412" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="B412" s="10" t="s">
+      <c r="B412" s="8" t="s">
         <v>987</v>
       </c>
       <c r="C412" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D412" s="11" t="s">
+      <c r="D412" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E412" s="11" t="s">
+      <c r="E412" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F412" s="0" t="n">
+      <c r="F412" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -11988,19 +12265,19 @@
       <c r="A413" s="1" t="s">
         <v>988</v>
       </c>
-      <c r="B413" s="10" t="s">
+      <c r="B413" s="8" t="s">
         <v>989</v>
       </c>
       <c r="C413" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D413" s="11" t="s">
+      <c r="D413" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E413" s="11" t="s">
+      <c r="E413" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F413" s="0" t="n">
+      <c r="F413" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12008,19 +12285,19 @@
       <c r="A414" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="B414" s="10" t="s">
+      <c r="B414" s="8" t="s">
         <v>991</v>
       </c>
       <c r="C414" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D414" s="11" t="s">
+      <c r="D414" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E414" s="11" t="s">
+      <c r="E414" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F414" s="0" t="n">
+      <c r="F414" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12028,19 +12305,19 @@
       <c r="A415" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B415" s="10" t="s">
+      <c r="B415" s="8" t="s">
         <v>993</v>
       </c>
       <c r="C415" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D415" s="11" t="s">
+      <c r="D415" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E415" s="11" t="s">
+      <c r="E415" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F415" s="0" t="n">
+      <c r="F415" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12048,19 +12325,19 @@
       <c r="A416" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B416" s="10" t="s">
+      <c r="B416" s="8" t="s">
         <v>995</v>
       </c>
       <c r="C416" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D416" s="11" t="s">
+      <c r="D416" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E416" s="11" t="s">
+      <c r="E416" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F416" s="0" t="n">
+      <c r="F416" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12068,19 +12345,19 @@
       <c r="A417" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="B417" s="10" t="s">
+      <c r="B417" s="8" t="s">
         <v>997</v>
       </c>
       <c r="C417" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D417" s="11" t="s">
+      <c r="D417" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="E417" s="11" t="s">
+      <c r="E417" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="F417" s="0" t="n">
+      <c r="F417" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12088,16 +12365,16 @@
       <c r="A418" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B418" s="10" t="s">
+      <c r="B418" s="8" t="s">
         <v>999</v>
       </c>
       <c r="C418" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E418" s="11" t="s">
+      <c r="E418" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="F418" s="0" t="n">
+      <c r="F418" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12105,19 +12382,19 @@
       <c r="A419" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="B419" s="10" t="s">
+      <c r="B419" s="8" t="s">
         <v>1001</v>
       </c>
       <c r="C419" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D419" s="11" t="s">
+      <c r="D419" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="E419" s="11" t="s">
+      <c r="E419" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F419" s="0" t="n">
+      <c r="F419" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12125,19 +12402,19 @@
       <c r="A420" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="B420" s="10" t="s">
+      <c r="B420" s="8" t="s">
         <v>1003</v>
       </c>
       <c r="C420" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D420" s="11" t="s">
+      <c r="D420" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E420" s="11" t="s">
+      <c r="E420" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F420" s="0" t="n">
+      <c r="F420" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12145,19 +12422,19 @@
       <c r="A421" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="B421" s="10" t="s">
+      <c r="B421" s="8" t="s">
         <v>1005</v>
       </c>
       <c r="C421" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D421" s="11" t="s">
+      <c r="D421" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E421" s="11" t="s">
+      <c r="E421" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="F421" s="0" t="n">
+      <c r="F421" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12165,19 +12442,19 @@
       <c r="A422" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="B422" s="10" t="s">
+      <c r="B422" s="8" t="s">
         <v>1007</v>
       </c>
       <c r="C422" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D422" s="11" t="s">
+      <c r="D422" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="E422" s="11" t="s">
+      <c r="E422" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F422" s="0" t="n">
+      <c r="F422" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12185,19 +12462,19 @@
       <c r="A423" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="B423" s="10" t="s">
+      <c r="B423" s="8" t="s">
         <v>1009</v>
       </c>
       <c r="C423" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D423" s="11" t="s">
+      <c r="D423" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="E423" s="11" t="s">
+      <c r="E423" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="F423" s="0" t="n">
+      <c r="F423" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12205,19 +12482,19 @@
       <c r="A424" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="B424" s="10" t="s">
+      <c r="B424" s="8" t="s">
         <v>1011</v>
       </c>
       <c r="C424" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D424" s="11" t="s">
+      <c r="D424" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E424" s="11" t="s">
+      <c r="E424" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F424" s="0" t="n">
+      <c r="F424" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12225,19 +12502,19 @@
       <c r="A425" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="B425" s="10" t="s">
+      <c r="B425" s="8" t="s">
         <v>1013</v>
       </c>
       <c r="C425" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D425" s="11" t="s">
+      <c r="D425" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E425" s="11" t="s">
+      <c r="E425" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F425" s="0" t="n">
+      <c r="F425" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12245,19 +12522,19 @@
       <c r="A426" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="B426" s="10" t="s">
+      <c r="B426" s="8" t="s">
         <v>1015</v>
       </c>
       <c r="C426" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D426" s="11" t="s">
+      <c r="D426" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E426" s="11" t="s">
+      <c r="E426" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F426" s="0" t="n">
+      <c r="F426" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12265,19 +12542,19 @@
       <c r="A427" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="B427" s="10" t="s">
+      <c r="B427" s="8" t="s">
         <v>1017</v>
       </c>
       <c r="C427" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D427" s="11" t="s">
+      <c r="D427" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E427" s="11" t="s">
+      <c r="E427" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F427" s="0" t="n">
+      <c r="F427" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12285,19 +12562,19 @@
       <c r="A428" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="B428" s="10" t="s">
+      <c r="B428" s="8" t="s">
         <v>1019</v>
       </c>
       <c r="C428" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D428" s="11" t="s">
+      <c r="D428" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E428" s="11" t="s">
+      <c r="E428" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="F428" s="0" t="n">
+      <c r="F428" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12305,16 +12582,16 @@
       <c r="A429" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="B429" s="10" t="s">
+      <c r="B429" s="8" t="s">
         <v>1021</v>
       </c>
       <c r="C429" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E429" s="11" t="s">
+      <c r="E429" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F429" s="0" t="n">
+      <c r="F429" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12322,19 +12599,19 @@
       <c r="A430" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="B430" s="10" t="s">
+      <c r="B430" s="8" t="s">
         <v>1023</v>
       </c>
       <c r="C430" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D430" s="11" t="s">
+      <c r="D430" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E430" s="11" t="s">
+      <c r="E430" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F430" s="0" t="n">
+      <c r="F430" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12342,19 +12619,19 @@
       <c r="A431" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="B431" s="10" t="s">
+      <c r="B431" s="8" t="s">
         <v>1025</v>
       </c>
       <c r="C431" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D431" s="11" t="s">
+      <c r="D431" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E431" s="11" t="s">
+      <c r="E431" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F431" s="0" t="n">
+      <c r="F431" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12362,19 +12639,19 @@
       <c r="A432" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="B432" s="10" t="s">
+      <c r="B432" s="8" t="s">
         <v>1027</v>
       </c>
       <c r="C432" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D432" s="11" t="s">
+      <c r="D432" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="E432" s="11" t="s">
+      <c r="E432" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="F432" s="0" t="n">
+      <c r="F432" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12382,19 +12659,19 @@
       <c r="A433" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="B433" s="10" t="s">
+      <c r="B433" s="8" t="s">
         <v>1029</v>
       </c>
       <c r="C433" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D433" s="11" t="s">
+      <c r="D433" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="E433" s="11" t="s">
+      <c r="E433" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="F433" s="0" t="n">
+      <c r="F433" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12402,19 +12679,19 @@
       <c r="A434" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B434" s="10" t="s">
+      <c r="B434" s="8" t="s">
         <v>1031</v>
       </c>
       <c r="C434" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D434" s="11" t="s">
+      <c r="D434" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E434" s="11" t="s">
+      <c r="E434" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F434" s="0" t="n">
+      <c r="F434" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12422,19 +12699,19 @@
       <c r="A435" s="1" t="s">
         <v>1032</v>
       </c>
-      <c r="B435" s="10" t="s">
+      <c r="B435" s="8" t="s">
         <v>1033</v>
       </c>
       <c r="C435" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D435" s="11" t="s">
+      <c r="D435" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E435" s="11" t="s">
+      <c r="E435" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="F435" s="0" t="n">
+      <c r="F435" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12442,19 +12719,19 @@
       <c r="A436" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="B436" s="10" t="s">
+      <c r="B436" s="8" t="s">
         <v>1035</v>
       </c>
       <c r="C436" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D436" s="11" t="s">
+      <c r="D436" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="E436" s="11" t="s">
+      <c r="E436" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="F436" s="0" t="n">
+      <c r="F436" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12462,16 +12739,16 @@
       <c r="A437" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="B437" s="10" t="s">
+      <c r="B437" s="8" t="s">
         <v>1037</v>
       </c>
       <c r="C437" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E437" s="11" t="s">
+      <c r="E437" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F437" s="0" t="n">
+      <c r="F437" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12479,19 +12756,19 @@
       <c r="A438" s="1" t="s">
         <v>1038</v>
       </c>
-      <c r="B438" s="10" t="s">
+      <c r="B438" s="8" t="s">
         <v>1039</v>
       </c>
       <c r="C438" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D438" s="11" t="s">
+      <c r="D438" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E438" s="11" t="s">
+      <c r="E438" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F438" s="0" t="n">
+      <c r="F438" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12499,19 +12776,19 @@
       <c r="A439" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="B439" s="10" t="s">
+      <c r="B439" s="8" t="s">
         <v>1041</v>
       </c>
       <c r="C439" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D439" s="11" t="s">
+      <c r="D439" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E439" s="11" t="s">
+      <c r="E439" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F439" s="0" t="n">
+      <c r="F439" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12519,19 +12796,19 @@
       <c r="A440" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B440" s="10" t="s">
+      <c r="B440" s="8" t="s">
         <v>1043</v>
       </c>
       <c r="C440" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="D440" s="11" t="s">
+      <c r="D440" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E440" s="11" t="s">
+      <c r="E440" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F440" s="0" t="n">
+      <c r="F440" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -12539,19 +12816,878 @@
       <c r="A441" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="B441" s="10" t="s">
+      <c r="B441" s="8" t="s">
         <v>1045</v>
       </c>
       <c r="C441" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D441" s="11" t="s">
+      <c r="D441" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="E441" s="11" t="s">
+      <c r="E441" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F441" s="0" t="n">
+      <c r="F441" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A442" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B442" s="8" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C442" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D442" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E442" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F442" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A443" s="8" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B443" s="8" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C443" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E443" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F443" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A444" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B444" s="8" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C444" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D444" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E444" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="F444" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A445" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B445" s="8" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C445" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D445" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E445" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F445" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A446" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B446" s="8" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C446" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D446" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="E446" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F446" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A447" s="8" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B447" s="8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C447" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D447" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E447" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F447" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A448" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B448" s="10" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C448" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D448" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E448" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F448" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A449" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B449" s="10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C449" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D449" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E449" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F449" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A450" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B450" s="10" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C450" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D450" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E450" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F450" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A451" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B451" s="10" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C451" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D451" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="E451" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F451" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A452" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B452" s="10" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C452" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D452" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E452" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F452" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A453" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B453" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C453" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D453" s="11" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E453" s="11" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F453" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A454" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B454" s="10" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C454" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D454" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E454" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F454" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A455" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B455" s="10" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C455" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E455" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F455" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A456" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B456" s="10" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C456" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D456" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E456" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F456" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A457" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B457" s="10" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C457" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D457" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E457" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F457" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A458" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B458" s="10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C458" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D458" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E458" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F458" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A459" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B459" s="10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C459" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D459" s="11" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E459" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="F459" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A460" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B460" s="10" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C460" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D460" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E460" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F460" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A461" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B461" s="10" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C461" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D461" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="E461" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F461" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A462" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B462" s="10" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C462" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D462" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="E462" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="F462" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A463" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B463" s="10" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C463" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D463" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="E463" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F463" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A464" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B464" s="10" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C464" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E464" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="F464" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A465" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B465" s="10" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C465" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D465" s="11" t="s">
+        <v>676</v>
+      </c>
+      <c r="E465" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F465" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A466" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B466" s="10" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C466" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D466" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E466" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F466" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A467" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B467" s="10" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C467" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D467" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E467" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F467" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A468" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B468" s="10" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C468" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E468" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F468" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A469" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B469" s="10" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C469" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D469" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E469" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F469" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A470" s="10" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B470" s="10" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C470" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D470" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E470" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F470" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A471" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B471" s="10" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C471" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D471" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E471" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="F471" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A472" s="10" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B472" s="10" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C472" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E472" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F472" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A473" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B473" s="10" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C473" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E473" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F473" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B474" s="10" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C474" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D474" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E474" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="F474" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A475" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B475" s="10" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C475" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D475" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E475" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F475" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A476" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B476" s="10" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C476" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E476" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F476" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A477" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B477" s="10" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C477" s="12" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D477" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E477" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F477" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A478" s="10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B478" s="10" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C478" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D478" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="E478" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="F478" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B479" s="10" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C479" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D479" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E479" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F479" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B480" s="10" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C480" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D480" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="E480" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F480" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A481" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B481" s="10" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C481" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D481" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="E481" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="F481" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A482" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B482" s="10" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C482" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D482" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E482" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F482" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A483" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B483" s="10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C483" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D483" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E483" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F483" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A484" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B484" s="10" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C484" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D484" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E484" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F484" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A485" s="10" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B485" s="10" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C485" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D485" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E485" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F485" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>